<commit_message>
done proj3 part 7
</commit_message>
<xml_diff>
--- a/61c-proj3/fa24-proj3-starter/[61C FA24] Project 3B ROM Control Logic.xlsx
+++ b/61c-proj3/fa24-proj3-starter/[61C FA24] Project 3B ROM Control Logic.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Courses\UCB CS61C 2024Fall\61c-proj3\fa24-proj3-starter\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34BFC57C-A1F7-4F84-B423-000FFDEAD4F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{736673C7-30B7-4E91-9113-59ED4F355C49}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="14295" yWindow="0" windowWidth="14610" windowHeight="15585" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -145,7 +145,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="304" uniqueCount="115">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="346" uniqueCount="117">
   <si>
     <t>MAKE A COPY OF THIS SHEET</t>
   </si>
@@ -505,6 +505,14 @@
   </si>
   <si>
     <t>01</t>
+    <phoneticPr fontId="13" type="noConversion"/>
+  </si>
+  <si>
+    <t>010</t>
+    <phoneticPr fontId="13" type="noConversion"/>
+  </si>
+  <si>
+    <t>00</t>
     <phoneticPr fontId="13" type="noConversion"/>
   </si>
 </sst>
@@ -742,10 +750,20 @@
     <xf numFmtId="0" fontId="11" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="49" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -759,16 +777,6 @@
     <xf numFmtId="49" fontId="4" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
@@ -999,10 +1007,10 @@
   <dimension ref="A1:W40"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="4" topLeftCell="B11" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="4" topLeftCell="H13" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="I31" sqref="I31"/>
+      <selection pane="bottomRight" activeCell="P5" sqref="P5:P40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1019,60 +1027,60 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="27" t="s">
+      <c r="A1" s="32" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="29" t="s">
+      <c r="B1" s="33" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="28"/>
-      <c r="D1" s="28"/>
-      <c r="E1" s="30"/>
-      <c r="F1" s="29" t="s">
+      <c r="C1" s="29"/>
+      <c r="D1" s="29"/>
+      <c r="E1" s="34"/>
+      <c r="F1" s="33" t="s">
         <v>2</v>
       </c>
-      <c r="G1" s="30"/>
-      <c r="H1" s="31" t="s">
+      <c r="G1" s="34"/>
+      <c r="H1" s="35" t="s">
         <v>3</v>
       </c>
-      <c r="I1" s="28"/>
-      <c r="J1" s="28"/>
-      <c r="K1" s="28"/>
-      <c r="L1" s="28"/>
-      <c r="M1" s="28"/>
-      <c r="N1" s="28"/>
-      <c r="O1" s="30"/>
+      <c r="I1" s="29"/>
+      <c r="J1" s="29"/>
+      <c r="K1" s="29"/>
+      <c r="L1" s="29"/>
+      <c r="M1" s="29"/>
+      <c r="N1" s="29"/>
+      <c r="O1" s="34"/>
       <c r="P1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="Q1" s="32" t="s">
+      <c r="Q1" s="36" t="s">
         <v>5</v>
       </c>
-      <c r="R1" s="28"/>
-      <c r="S1" s="28"/>
-      <c r="T1" s="28"/>
-      <c r="U1" s="28"/>
-      <c r="V1" s="28"/>
-      <c r="W1" s="28"/>
+      <c r="R1" s="29"/>
+      <c r="S1" s="29"/>
+      <c r="T1" s="29"/>
+      <c r="U1" s="29"/>
+      <c r="V1" s="29"/>
+      <c r="W1" s="29"/>
     </row>
     <row r="2" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="28"/>
+      <c r="A2" s="29"/>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
       <c r="D2" s="1"/>
       <c r="E2" s="4"/>
       <c r="F2" s="1"/>
       <c r="G2" s="4"/>
-      <c r="H2" s="33" t="s">
+      <c r="H2" s="37" t="s">
         <v>6</v>
       </c>
-      <c r="I2" s="28"/>
-      <c r="J2" s="28"/>
-      <c r="K2" s="28"/>
-      <c r="L2" s="28"/>
-      <c r="M2" s="28"/>
-      <c r="N2" s="28"/>
-      <c r="O2" s="30"/>
+      <c r="I2" s="29"/>
+      <c r="J2" s="29"/>
+      <c r="K2" s="29"/>
+      <c r="L2" s="29"/>
+      <c r="M2" s="29"/>
+      <c r="N2" s="29"/>
+      <c r="O2" s="34"/>
       <c r="P2" s="2"/>
       <c r="Q2" s="3"/>
       <c r="R2" s="3"/>
@@ -1082,7 +1090,7 @@
       <c r="V2" s="3"/>
       <c r="W2" s="3"/>
     </row>
-    <row r="3" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:23" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A3" s="5" t="s">
         <v>7</v>
       </c>
@@ -1153,7 +1161,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="4" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:23" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A4" s="5"/>
       <c r="B4" s="6"/>
       <c r="C4" s="6"/>
@@ -1198,10 +1206,10 @@
       <c r="A5" s="16" t="s">
         <v>33</v>
       </c>
-      <c r="B5" s="35" t="s">
+      <c r="B5" s="30" t="s">
         <v>34</v>
       </c>
-      <c r="C5" s="34" t="s">
+      <c r="C5" s="28" t="s">
         <v>35</v>
       </c>
       <c r="D5" s="17" t="s">
@@ -1218,28 +1226,28 @@
         <f t="shared" ref="G5:G40" si="0">V5</f>
         <v>0</v>
       </c>
-      <c r="H5" s="37" t="s">
-        <v>99</v>
-      </c>
-      <c r="I5" s="37" t="s">
+      <c r="H5" s="27" t="s">
+        <v>99</v>
+      </c>
+      <c r="I5" s="27" t="s">
         <v>100</v>
       </c>
-      <c r="J5" s="37" t="s">
-        <v>101</v>
-      </c>
-      <c r="K5" s="37" t="s">
-        <v>99</v>
-      </c>
-      <c r="L5" s="37" t="s">
-        <v>99</v>
-      </c>
-      <c r="M5" s="37" t="s">
+      <c r="J5" s="27" t="s">
+        <v>101</v>
+      </c>
+      <c r="K5" s="27" t="s">
+        <v>99</v>
+      </c>
+      <c r="L5" s="27" t="s">
+        <v>99</v>
+      </c>
+      <c r="M5" s="27" t="s">
         <v>102</v>
       </c>
-      <c r="N5" s="37" t="s">
-        <v>101</v>
-      </c>
-      <c r="O5" s="37" t="s">
+      <c r="N5" s="27" t="s">
+        <v>101</v>
+      </c>
+      <c r="O5" s="27" t="s">
         <v>114</v>
       </c>
       <c r="P5" s="11" t="str">
@@ -1278,8 +1286,8 @@
       <c r="A6" s="16" t="s">
         <v>38</v>
       </c>
-      <c r="B6" s="28"/>
-      <c r="C6" s="28"/>
+      <c r="B6" s="29"/>
+      <c r="C6" s="29"/>
       <c r="D6" s="17" t="s">
         <v>36</v>
       </c>
@@ -1294,28 +1302,28 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="H6" s="37" t="s">
-        <v>99</v>
-      </c>
-      <c r="I6" s="37" t="s">
+      <c r="H6" s="27" t="s">
+        <v>99</v>
+      </c>
+      <c r="I6" s="27" t="s">
         <v>100</v>
       </c>
-      <c r="J6" s="37" t="s">
-        <v>101</v>
-      </c>
-      <c r="K6" s="37" t="s">
-        <v>99</v>
-      </c>
-      <c r="L6" s="37" t="s">
-        <v>99</v>
-      </c>
-      <c r="M6" s="37" t="s">
+      <c r="J6" s="27" t="s">
+        <v>101</v>
+      </c>
+      <c r="K6" s="27" t="s">
+        <v>99</v>
+      </c>
+      <c r="L6" s="27" t="s">
+        <v>99</v>
+      </c>
+      <c r="M6" s="27" t="s">
         <v>103</v>
       </c>
-      <c r="N6" s="37" t="s">
-        <v>101</v>
-      </c>
-      <c r="O6" s="37" t="s">
+      <c r="N6" s="27" t="s">
+        <v>101</v>
+      </c>
+      <c r="O6" s="27" t="s">
         <v>114</v>
       </c>
       <c r="P6" s="11" t="str">
@@ -1354,8 +1362,8 @@
       <c r="A7" s="16" t="s">
         <v>40</v>
       </c>
-      <c r="B7" s="28"/>
-      <c r="C7" s="28"/>
+      <c r="B7" s="29"/>
+      <c r="C7" s="29"/>
       <c r="D7" s="17" t="s">
         <v>36</v>
       </c>
@@ -1370,28 +1378,28 @@
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
-      <c r="H7" s="37" t="s">
-        <v>99</v>
-      </c>
-      <c r="I7" s="37" t="s">
+      <c r="H7" s="27" t="s">
+        <v>99</v>
+      </c>
+      <c r="I7" s="27" t="s">
         <v>100</v>
       </c>
-      <c r="J7" s="37" t="s">
-        <v>101</v>
-      </c>
-      <c r="K7" s="37" t="s">
-        <v>99</v>
-      </c>
-      <c r="L7" s="37" t="s">
-        <v>99</v>
-      </c>
-      <c r="M7" s="37" t="s">
+      <c r="J7" s="27" t="s">
+        <v>101</v>
+      </c>
+      <c r="K7" s="27" t="s">
+        <v>99</v>
+      </c>
+      <c r="L7" s="27" t="s">
+        <v>99</v>
+      </c>
+      <c r="M7" s="27" t="s">
         <v>104</v>
       </c>
-      <c r="N7" s="37" t="s">
-        <v>101</v>
-      </c>
-      <c r="O7" s="37" t="s">
+      <c r="N7" s="27" t="s">
+        <v>101</v>
+      </c>
+      <c r="O7" s="27" t="s">
         <v>114</v>
       </c>
       <c r="P7" s="11" t="str">
@@ -1430,8 +1438,8 @@
       <c r="A8" s="16" t="s">
         <v>42</v>
       </c>
-      <c r="B8" s="28"/>
-      <c r="C8" s="28"/>
+      <c r="B8" s="29"/>
+      <c r="C8" s="29"/>
       <c r="D8" s="17" t="s">
         <v>43</v>
       </c>
@@ -1446,28 +1454,28 @@
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
-      <c r="H8" s="37" t="s">
-        <v>99</v>
-      </c>
-      <c r="I8" s="37" t="s">
+      <c r="H8" s="27" t="s">
+        <v>99</v>
+      </c>
+      <c r="I8" s="27" t="s">
         <v>100</v>
       </c>
-      <c r="J8" s="37" t="s">
-        <v>101</v>
-      </c>
-      <c r="K8" s="37" t="s">
-        <v>99</v>
-      </c>
-      <c r="L8" s="37" t="s">
-        <v>99</v>
-      </c>
-      <c r="M8" s="37" t="s">
+      <c r="J8" s="27" t="s">
+        <v>101</v>
+      </c>
+      <c r="K8" s="27" t="s">
+        <v>99</v>
+      </c>
+      <c r="L8" s="27" t="s">
+        <v>99</v>
+      </c>
+      <c r="M8" s="27" t="s">
         <v>105</v>
       </c>
-      <c r="N8" s="37" t="s">
-        <v>101</v>
-      </c>
-      <c r="O8" s="37" t="s">
+      <c r="N8" s="27" t="s">
+        <v>101</v>
+      </c>
+      <c r="O8" s="27" t="s">
         <v>114</v>
       </c>
       <c r="P8" s="11" t="str">
@@ -1506,8 +1514,8 @@
       <c r="A9" s="16" t="s">
         <v>44</v>
       </c>
-      <c r="B9" s="28"/>
-      <c r="C9" s="28"/>
+      <c r="B9" s="29"/>
+      <c r="C9" s="29"/>
       <c r="D9" s="20" t="s">
         <v>43</v>
       </c>
@@ -1522,28 +1530,28 @@
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="H9" s="37" t="s">
-        <v>99</v>
-      </c>
-      <c r="I9" s="37" t="s">
+      <c r="H9" s="27" t="s">
+        <v>99</v>
+      </c>
+      <c r="I9" s="27" t="s">
         <v>100</v>
       </c>
-      <c r="J9" s="37" t="s">
-        <v>101</v>
-      </c>
-      <c r="K9" s="37" t="s">
-        <v>99</v>
-      </c>
-      <c r="L9" s="37" t="s">
-        <v>99</v>
-      </c>
-      <c r="M9" s="37" t="s">
+      <c r="J9" s="27" t="s">
+        <v>101</v>
+      </c>
+      <c r="K9" s="27" t="s">
+        <v>99</v>
+      </c>
+      <c r="L9" s="27" t="s">
+        <v>99</v>
+      </c>
+      <c r="M9" s="27" t="s">
         <v>106</v>
       </c>
-      <c r="N9" s="37" t="s">
-        <v>101</v>
-      </c>
-      <c r="O9" s="37" t="s">
+      <c r="N9" s="27" t="s">
+        <v>101</v>
+      </c>
+      <c r="O9" s="27" t="s">
         <v>114</v>
       </c>
       <c r="P9" s="11" t="str">
@@ -1582,8 +1590,8 @@
       <c r="A10" s="16" t="s">
         <v>45</v>
       </c>
-      <c r="B10" s="28"/>
-      <c r="C10" s="28"/>
+      <c r="B10" s="29"/>
+      <c r="C10" s="29"/>
       <c r="D10" s="17" t="s">
         <v>46</v>
       </c>
@@ -1598,28 +1606,28 @@
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="H10" s="37" t="s">
-        <v>99</v>
-      </c>
-      <c r="I10" s="37" t="s">
+      <c r="H10" s="27" t="s">
+        <v>99</v>
+      </c>
+      <c r="I10" s="27" t="s">
         <v>100</v>
       </c>
-      <c r="J10" s="37" t="s">
-        <v>101</v>
-      </c>
-      <c r="K10" s="37" t="s">
-        <v>99</v>
-      </c>
-      <c r="L10" s="37" t="s">
-        <v>99</v>
-      </c>
-      <c r="M10" s="37" t="s">
+      <c r="J10" s="27" t="s">
+        <v>101</v>
+      </c>
+      <c r="K10" s="27" t="s">
+        <v>99</v>
+      </c>
+      <c r="L10" s="27" t="s">
+        <v>99</v>
+      </c>
+      <c r="M10" s="27" t="s">
         <v>107</v>
       </c>
-      <c r="N10" s="37" t="s">
-        <v>101</v>
-      </c>
-      <c r="O10" s="37" t="s">
+      <c r="N10" s="27" t="s">
+        <v>101</v>
+      </c>
+      <c r="O10" s="27" t="s">
         <v>114</v>
       </c>
       <c r="P10" s="11" t="str">
@@ -1658,8 +1666,8 @@
       <c r="A11" s="16" t="s">
         <v>47</v>
       </c>
-      <c r="B11" s="28"/>
-      <c r="C11" s="28"/>
+      <c r="B11" s="29"/>
+      <c r="C11" s="29"/>
       <c r="D11" s="17" t="s">
         <v>48</v>
       </c>
@@ -1674,28 +1682,28 @@
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="H11" s="37" t="s">
-        <v>99</v>
-      </c>
-      <c r="I11" s="37" t="s">
+      <c r="H11" s="27" t="s">
+        <v>99</v>
+      </c>
+      <c r="I11" s="27" t="s">
         <v>100</v>
       </c>
-      <c r="J11" s="37" t="s">
-        <v>101</v>
-      </c>
-      <c r="K11" s="37" t="s">
-        <v>99</v>
-      </c>
-      <c r="L11" s="37" t="s">
-        <v>99</v>
-      </c>
-      <c r="M11" s="37" t="s">
+      <c r="J11" s="27" t="s">
+        <v>101</v>
+      </c>
+      <c r="K11" s="27" t="s">
+        <v>99</v>
+      </c>
+      <c r="L11" s="27" t="s">
+        <v>99</v>
+      </c>
+      <c r="M11" s="27" t="s">
         <v>108</v>
       </c>
-      <c r="N11" s="37" t="s">
-        <v>101</v>
-      </c>
-      <c r="O11" s="37" t="s">
+      <c r="N11" s="27" t="s">
+        <v>101</v>
+      </c>
+      <c r="O11" s="27" t="s">
         <v>114</v>
       </c>
       <c r="P11" s="11" t="str">
@@ -1734,8 +1742,8 @@
       <c r="A12" s="16" t="s">
         <v>49</v>
       </c>
-      <c r="B12" s="28"/>
-      <c r="C12" s="28"/>
+      <c r="B12" s="29"/>
+      <c r="C12" s="29"/>
       <c r="D12" s="17" t="s">
         <v>50</v>
       </c>
@@ -1750,28 +1758,28 @@
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
-      <c r="H12" s="37" t="s">
-        <v>99</v>
-      </c>
-      <c r="I12" s="37" t="s">
+      <c r="H12" s="27" t="s">
+        <v>99</v>
+      </c>
+      <c r="I12" s="27" t="s">
         <v>100</v>
       </c>
-      <c r="J12" s="37" t="s">
-        <v>101</v>
-      </c>
-      <c r="K12" s="37" t="s">
-        <v>99</v>
-      </c>
-      <c r="L12" s="37" t="s">
-        <v>99</v>
-      </c>
-      <c r="M12" s="37" t="s">
+      <c r="J12" s="27" t="s">
+        <v>101</v>
+      </c>
+      <c r="K12" s="27" t="s">
+        <v>99</v>
+      </c>
+      <c r="L12" s="27" t="s">
+        <v>99</v>
+      </c>
+      <c r="M12" s="27" t="s">
         <v>109</v>
       </c>
-      <c r="N12" s="37" t="s">
-        <v>101</v>
-      </c>
-      <c r="O12" s="37" t="s">
+      <c r="N12" s="27" t="s">
+        <v>101</v>
+      </c>
+      <c r="O12" s="27" t="s">
         <v>114</v>
       </c>
       <c r="P12" s="11" t="str">
@@ -1810,8 +1818,8 @@
       <c r="A13" s="16" t="s">
         <v>51</v>
       </c>
-      <c r="B13" s="28"/>
-      <c r="C13" s="28"/>
+      <c r="B13" s="29"/>
+      <c r="C13" s="29"/>
       <c r="D13" s="17" t="s">
         <v>52</v>
       </c>
@@ -1826,28 +1834,28 @@
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
-      <c r="H13" s="37" t="s">
-        <v>99</v>
-      </c>
-      <c r="I13" s="37" t="s">
+      <c r="H13" s="27" t="s">
+        <v>99</v>
+      </c>
+      <c r="I13" s="27" t="s">
         <v>100</v>
       </c>
-      <c r="J13" s="37" t="s">
-        <v>101</v>
-      </c>
-      <c r="K13" s="37" t="s">
-        <v>99</v>
-      </c>
-      <c r="L13" s="37" t="s">
-        <v>99</v>
-      </c>
-      <c r="M13" s="37" t="s">
+      <c r="J13" s="27" t="s">
+        <v>101</v>
+      </c>
+      <c r="K13" s="27" t="s">
+        <v>99</v>
+      </c>
+      <c r="L13" s="27" t="s">
+        <v>99</v>
+      </c>
+      <c r="M13" s="27" t="s">
         <v>110</v>
       </c>
-      <c r="N13" s="37" t="s">
-        <v>101</v>
-      </c>
-      <c r="O13" s="37" t="s">
+      <c r="N13" s="27" t="s">
+        <v>101</v>
+      </c>
+      <c r="O13" s="27" t="s">
         <v>114</v>
       </c>
       <c r="P13" s="11" t="str">
@@ -1886,8 +1894,8 @@
       <c r="A14" s="16" t="s">
         <v>53</v>
       </c>
-      <c r="B14" s="28"/>
-      <c r="C14" s="28"/>
+      <c r="B14" s="29"/>
+      <c r="C14" s="29"/>
       <c r="D14" s="17" t="s">
         <v>52</v>
       </c>
@@ -1902,28 +1910,28 @@
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
-      <c r="H14" s="37" t="s">
-        <v>99</v>
-      </c>
-      <c r="I14" s="37" t="s">
+      <c r="H14" s="27" t="s">
+        <v>99</v>
+      </c>
+      <c r="I14" s="27" t="s">
         <v>100</v>
       </c>
-      <c r="J14" s="37" t="s">
-        <v>101</v>
-      </c>
-      <c r="K14" s="37" t="s">
-        <v>99</v>
-      </c>
-      <c r="L14" s="37" t="s">
-        <v>99</v>
-      </c>
-      <c r="M14" s="37" t="s">
+      <c r="J14" s="27" t="s">
+        <v>101</v>
+      </c>
+      <c r="K14" s="27" t="s">
+        <v>99</v>
+      </c>
+      <c r="L14" s="27" t="s">
+        <v>99</v>
+      </c>
+      <c r="M14" s="27" t="s">
         <v>111</v>
       </c>
-      <c r="N14" s="37" t="s">
-        <v>101</v>
-      </c>
-      <c r="O14" s="37" t="s">
+      <c r="N14" s="27" t="s">
+        <v>101</v>
+      </c>
+      <c r="O14" s="27" t="s">
         <v>114</v>
       </c>
       <c r="P14" s="11" t="str">
@@ -1962,8 +1970,8 @@
       <c r="A15" s="16" t="s">
         <v>54</v>
       </c>
-      <c r="B15" s="28"/>
-      <c r="C15" s="28"/>
+      <c r="B15" s="29"/>
+      <c r="C15" s="29"/>
       <c r="D15" s="17" t="s">
         <v>55</v>
       </c>
@@ -1978,28 +1986,28 @@
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-      <c r="H15" s="37" t="s">
-        <v>99</v>
-      </c>
-      <c r="I15" s="37" t="s">
+      <c r="H15" s="27" t="s">
+        <v>99</v>
+      </c>
+      <c r="I15" s="27" t="s">
         <v>100</v>
       </c>
-      <c r="J15" s="37" t="s">
-        <v>101</v>
-      </c>
-      <c r="K15" s="37" t="s">
-        <v>99</v>
-      </c>
-      <c r="L15" s="37" t="s">
-        <v>99</v>
-      </c>
-      <c r="M15" s="37" t="s">
+      <c r="J15" s="27" t="s">
+        <v>101</v>
+      </c>
+      <c r="K15" s="27" t="s">
+        <v>99</v>
+      </c>
+      <c r="L15" s="27" t="s">
+        <v>99</v>
+      </c>
+      <c r="M15" s="27" t="s">
         <v>112</v>
       </c>
-      <c r="N15" s="37" t="s">
-        <v>101</v>
-      </c>
-      <c r="O15" s="37" t="s">
+      <c r="N15" s="27" t="s">
+        <v>101</v>
+      </c>
+      <c r="O15" s="27" t="s">
         <v>114</v>
       </c>
       <c r="P15" s="11" t="str">
@@ -2038,8 +2046,8 @@
       <c r="A16" s="16" t="s">
         <v>56</v>
       </c>
-      <c r="B16" s="28"/>
-      <c r="C16" s="28"/>
+      <c r="B16" s="29"/>
+      <c r="C16" s="29"/>
       <c r="D16" s="17" t="s">
         <v>57</v>
       </c>
@@ -2054,28 +2062,28 @@
         <f t="shared" si="0"/>
         <v>11</v>
       </c>
-      <c r="H16" s="37" t="s">
-        <v>99</v>
-      </c>
-      <c r="I16" s="37" t="s">
+      <c r="H16" s="27" t="s">
+        <v>99</v>
+      </c>
+      <c r="I16" s="27" t="s">
         <v>100</v>
       </c>
-      <c r="J16" s="37" t="s">
-        <v>101</v>
-      </c>
-      <c r="K16" s="37" t="s">
-        <v>99</v>
-      </c>
-      <c r="L16" s="37" t="s">
-        <v>99</v>
-      </c>
-      <c r="M16" s="37" t="s">
+      <c r="J16" s="27" t="s">
+        <v>101</v>
+      </c>
+      <c r="K16" s="27" t="s">
+        <v>99</v>
+      </c>
+      <c r="L16" s="27" t="s">
+        <v>99</v>
+      </c>
+      <c r="M16" s="27" t="s">
         <v>113</v>
       </c>
-      <c r="N16" s="37" t="s">
-        <v>101</v>
-      </c>
-      <c r="O16" s="37" t="s">
+      <c r="N16" s="27" t="s">
+        <v>101</v>
+      </c>
+      <c r="O16" s="27" t="s">
         <v>114</v>
       </c>
       <c r="P16" s="11" t="str">
@@ -2114,10 +2122,10 @@
       <c r="A17" s="16" t="s">
         <v>58</v>
       </c>
-      <c r="B17" s="35" t="s">
+      <c r="B17" s="30" t="s">
         <v>59</v>
       </c>
-      <c r="C17" s="36" t="s">
+      <c r="C17" s="31" t="s">
         <v>60</v>
       </c>
       <c r="D17" s="17" t="s">
@@ -2176,8 +2184,8 @@
       <c r="A18" s="16" t="s">
         <v>61</v>
       </c>
-      <c r="B18" s="28"/>
-      <c r="C18" s="28"/>
+      <c r="B18" s="29"/>
+      <c r="C18" s="29"/>
       <c r="D18" s="20" t="s">
         <v>43</v>
       </c>
@@ -2234,8 +2242,8 @@
       <c r="A19" s="16" t="s">
         <v>62</v>
       </c>
-      <c r="B19" s="28"/>
-      <c r="C19" s="28"/>
+      <c r="B19" s="29"/>
+      <c r="C19" s="29"/>
       <c r="D19" s="17" t="s">
         <v>48</v>
       </c>
@@ -2292,8 +2300,8 @@
       <c r="A20" s="16" t="s">
         <v>63</v>
       </c>
-      <c r="B20" s="28"/>
-      <c r="C20" s="36" t="s">
+      <c r="B20" s="29"/>
+      <c r="C20" s="31" t="s">
         <v>64</v>
       </c>
       <c r="D20" s="17" t="s">
@@ -2311,16 +2319,16 @@
       <c r="H20" s="24" t="s">
         <v>65</v>
       </c>
-      <c r="I20" s="37" t="s">
+      <c r="I20" s="27" t="s">
         <v>100</v>
       </c>
       <c r="J20" s="19" t="s">
         <v>66</v>
       </c>
-      <c r="K20" s="37" t="s">
-        <v>99</v>
-      </c>
-      <c r="L20" s="37" t="s">
+      <c r="K20" s="27" t="s">
+        <v>99</v>
+      </c>
+      <c r="L20" s="27" t="s">
         <v>101</v>
       </c>
       <c r="M20" s="19" t="s">
@@ -2368,8 +2376,8 @@
       <c r="A21" s="16" t="s">
         <v>69</v>
       </c>
-      <c r="B21" s="28"/>
-      <c r="C21" s="28"/>
+      <c r="B21" s="29"/>
+      <c r="C21" s="29"/>
       <c r="D21" s="20" t="s">
         <v>43</v>
       </c>
@@ -2384,28 +2392,28 @@
         <f t="shared" si="0"/>
         <v>16</v>
       </c>
-      <c r="H21" s="37" t="s">
-        <v>99</v>
-      </c>
-      <c r="I21" s="37" t="s">
+      <c r="H21" s="27" t="s">
+        <v>99</v>
+      </c>
+      <c r="I21" s="27" t="s">
         <v>100</v>
       </c>
-      <c r="J21" s="37" t="s">
-        <v>101</v>
-      </c>
-      <c r="K21" s="37" t="s">
-        <v>99</v>
-      </c>
-      <c r="L21" s="37" t="s">
-        <v>101</v>
-      </c>
-      <c r="M21" s="37" t="s">
+      <c r="J21" s="27" t="s">
+        <v>101</v>
+      </c>
+      <c r="K21" s="27" t="s">
+        <v>99</v>
+      </c>
+      <c r="L21" s="27" t="s">
+        <v>101</v>
+      </c>
+      <c r="M21" s="27" t="s">
         <v>105</v>
       </c>
-      <c r="N21" s="37" t="s">
-        <v>101</v>
-      </c>
-      <c r="O21" s="37" t="s">
+      <c r="N21" s="27" t="s">
+        <v>101</v>
+      </c>
+      <c r="O21" s="27" t="s">
         <v>114</v>
       </c>
       <c r="P21" s="11" t="str">
@@ -2444,8 +2452,8 @@
       <c r="A22" s="16" t="s">
         <v>70</v>
       </c>
-      <c r="B22" s="28"/>
-      <c r="C22" s="28"/>
+      <c r="B22" s="29"/>
+      <c r="C22" s="29"/>
       <c r="D22" s="17" t="s">
         <v>48</v>
       </c>
@@ -2458,28 +2466,28 @@
         <f t="shared" si="0"/>
         <v>17</v>
       </c>
-      <c r="H22" s="37" t="s">
-        <v>99</v>
-      </c>
-      <c r="I22" s="37" t="s">
+      <c r="H22" s="27" t="s">
+        <v>99</v>
+      </c>
+      <c r="I22" s="27" t="s">
         <v>100</v>
       </c>
-      <c r="J22" s="37" t="s">
-        <v>101</v>
-      </c>
-      <c r="K22" s="37" t="s">
-        <v>99</v>
-      </c>
-      <c r="L22" s="37" t="s">
-        <v>101</v>
-      </c>
-      <c r="M22" s="37" t="s">
+      <c r="J22" s="27" t="s">
+        <v>101</v>
+      </c>
+      <c r="K22" s="27" t="s">
+        <v>99</v>
+      </c>
+      <c r="L22" s="27" t="s">
+        <v>101</v>
+      </c>
+      <c r="M22" s="27" t="s">
         <v>108</v>
       </c>
-      <c r="N22" s="37" t="s">
-        <v>101</v>
-      </c>
-      <c r="O22" s="37" t="s">
+      <c r="N22" s="27" t="s">
+        <v>101</v>
+      </c>
+      <c r="O22" s="27" t="s">
         <v>114</v>
       </c>
       <c r="P22" s="11" t="str">
@@ -2518,8 +2526,8 @@
       <c r="A23" s="16" t="s">
         <v>71</v>
       </c>
-      <c r="B23" s="28"/>
-      <c r="C23" s="28"/>
+      <c r="B23" s="29"/>
+      <c r="C23" s="29"/>
       <c r="D23" s="20" t="s">
         <v>50</v>
       </c>
@@ -2532,28 +2540,28 @@
         <f t="shared" si="0"/>
         <v>18</v>
       </c>
-      <c r="H23" s="37" t="s">
-        <v>99</v>
-      </c>
-      <c r="I23" s="37" t="s">
+      <c r="H23" s="27" t="s">
+        <v>99</v>
+      </c>
+      <c r="I23" s="27" t="s">
         <v>100</v>
       </c>
-      <c r="J23" s="37" t="s">
-        <v>101</v>
-      </c>
-      <c r="K23" s="37" t="s">
-        <v>99</v>
-      </c>
-      <c r="L23" s="37" t="s">
-        <v>101</v>
-      </c>
-      <c r="M23" s="37" t="s">
+      <c r="J23" s="27" t="s">
+        <v>101</v>
+      </c>
+      <c r="K23" s="27" t="s">
+        <v>99</v>
+      </c>
+      <c r="L23" s="27" t="s">
+        <v>101</v>
+      </c>
+      <c r="M23" s="27" t="s">
         <v>109</v>
       </c>
-      <c r="N23" s="37" t="s">
-        <v>101</v>
-      </c>
-      <c r="O23" s="37" t="s">
+      <c r="N23" s="27" t="s">
+        <v>101</v>
+      </c>
+      <c r="O23" s="27" t="s">
         <v>114</v>
       </c>
       <c r="P23" s="11" t="str">
@@ -2592,8 +2600,8 @@
       <c r="A24" s="16" t="s">
         <v>72</v>
       </c>
-      <c r="B24" s="28"/>
-      <c r="C24" s="28"/>
+      <c r="B24" s="29"/>
+      <c r="C24" s="29"/>
       <c r="D24" s="17" t="s">
         <v>52</v>
       </c>
@@ -2608,28 +2616,28 @@
         <f t="shared" si="0"/>
         <v>19</v>
       </c>
-      <c r="H24" s="37" t="s">
-        <v>99</v>
-      </c>
-      <c r="I24" s="37" t="s">
+      <c r="H24" s="27" t="s">
+        <v>99</v>
+      </c>
+      <c r="I24" s="27" t="s">
         <v>100</v>
       </c>
-      <c r="J24" s="37" t="s">
-        <v>101</v>
-      </c>
-      <c r="K24" s="37" t="s">
-        <v>99</v>
-      </c>
-      <c r="L24" s="37" t="s">
-        <v>101</v>
-      </c>
-      <c r="M24" s="37" t="s">
+      <c r="J24" s="27" t="s">
+        <v>101</v>
+      </c>
+      <c r="K24" s="27" t="s">
+        <v>99</v>
+      </c>
+      <c r="L24" s="27" t="s">
+        <v>101</v>
+      </c>
+      <c r="M24" s="27" t="s">
         <v>110</v>
       </c>
-      <c r="N24" s="37" t="s">
-        <v>101</v>
-      </c>
-      <c r="O24" s="37" t="s">
+      <c r="N24" s="27" t="s">
+        <v>101</v>
+      </c>
+      <c r="O24" s="27" t="s">
         <v>114</v>
       </c>
       <c r="P24" s="11" t="str">
@@ -2668,8 +2676,8 @@
       <c r="A25" s="16" t="s">
         <v>73</v>
       </c>
-      <c r="B25" s="28"/>
-      <c r="C25" s="28"/>
+      <c r="B25" s="29"/>
+      <c r="C25" s="29"/>
       <c r="D25" s="17" t="s">
         <v>52</v>
       </c>
@@ -2684,28 +2692,28 @@
         <f t="shared" si="0"/>
         <v>20</v>
       </c>
-      <c r="H25" s="37" t="s">
-        <v>99</v>
-      </c>
-      <c r="I25" s="37" t="s">
+      <c r="H25" s="27" t="s">
+        <v>99</v>
+      </c>
+      <c r="I25" s="27" t="s">
         <v>100</v>
       </c>
-      <c r="J25" s="37" t="s">
-        <v>101</v>
-      </c>
-      <c r="K25" s="37" t="s">
-        <v>99</v>
-      </c>
-      <c r="L25" s="37" t="s">
-        <v>101</v>
-      </c>
-      <c r="M25" s="37" t="s">
+      <c r="J25" s="27" t="s">
+        <v>101</v>
+      </c>
+      <c r="K25" s="27" t="s">
+        <v>99</v>
+      </c>
+      <c r="L25" s="27" t="s">
+        <v>101</v>
+      </c>
+      <c r="M25" s="27" t="s">
         <v>111</v>
       </c>
-      <c r="N25" s="37" t="s">
-        <v>101</v>
-      </c>
-      <c r="O25" s="37" t="s">
+      <c r="N25" s="27" t="s">
+        <v>101</v>
+      </c>
+      <c r="O25" s="27" t="s">
         <v>114</v>
       </c>
       <c r="P25" s="11" t="str">
@@ -2744,8 +2752,8 @@
       <c r="A26" s="16" t="s">
         <v>74</v>
       </c>
-      <c r="B26" s="28"/>
-      <c r="C26" s="28"/>
+      <c r="B26" s="29"/>
+      <c r="C26" s="29"/>
       <c r="D26" s="17" t="s">
         <v>55</v>
       </c>
@@ -2758,28 +2766,28 @@
         <f t="shared" si="0"/>
         <v>21</v>
       </c>
-      <c r="H26" s="37" t="s">
-        <v>99</v>
-      </c>
-      <c r="I26" s="37" t="s">
+      <c r="H26" s="27" t="s">
+        <v>99</v>
+      </c>
+      <c r="I26" s="27" t="s">
         <v>100</v>
       </c>
-      <c r="J26" s="37" t="s">
-        <v>101</v>
-      </c>
-      <c r="K26" s="37" t="s">
-        <v>99</v>
-      </c>
-      <c r="L26" s="37" t="s">
-        <v>101</v>
-      </c>
-      <c r="M26" s="37" t="s">
+      <c r="J26" s="27" t="s">
+        <v>101</v>
+      </c>
+      <c r="K26" s="27" t="s">
+        <v>99</v>
+      </c>
+      <c r="L26" s="27" t="s">
+        <v>101</v>
+      </c>
+      <c r="M26" s="27" t="s">
         <v>112</v>
       </c>
-      <c r="N26" s="37" t="s">
-        <v>101</v>
-      </c>
-      <c r="O26" s="37" t="s">
+      <c r="N26" s="27" t="s">
+        <v>101</v>
+      </c>
+      <c r="O26" s="27" t="s">
         <v>114</v>
       </c>
       <c r="P26" s="11" t="str">
@@ -2818,8 +2826,8 @@
       <c r="A27" s="16" t="s">
         <v>75</v>
       </c>
-      <c r="B27" s="28"/>
-      <c r="C27" s="28"/>
+      <c r="B27" s="29"/>
+      <c r="C27" s="29"/>
       <c r="D27" s="17" t="s">
         <v>57</v>
       </c>
@@ -2832,28 +2840,28 @@
         <f t="shared" si="0"/>
         <v>22</v>
       </c>
-      <c r="H27" s="37" t="s">
-        <v>99</v>
-      </c>
-      <c r="I27" s="37" t="s">
+      <c r="H27" s="27" t="s">
+        <v>99</v>
+      </c>
+      <c r="I27" s="27" t="s">
         <v>100</v>
       </c>
-      <c r="J27" s="37" t="s">
-        <v>101</v>
-      </c>
-      <c r="K27" s="37" t="s">
-        <v>99</v>
-      </c>
-      <c r="L27" s="37" t="s">
-        <v>101</v>
-      </c>
-      <c r="M27" s="37" t="s">
+      <c r="J27" s="27" t="s">
+        <v>101</v>
+      </c>
+      <c r="K27" s="27" t="s">
+        <v>99</v>
+      </c>
+      <c r="L27" s="27" t="s">
+        <v>101</v>
+      </c>
+      <c r="M27" s="27" t="s">
         <v>113</v>
       </c>
-      <c r="N27" s="37" t="s">
-        <v>101</v>
-      </c>
-      <c r="O27" s="37" t="s">
+      <c r="N27" s="27" t="s">
+        <v>101</v>
+      </c>
+      <c r="O27" s="27" t="s">
         <v>114</v>
       </c>
       <c r="P27" s="11" t="str">
@@ -2892,10 +2900,10 @@
       <c r="A28" s="16" t="s">
         <v>76</v>
       </c>
-      <c r="B28" s="35" t="s">
+      <c r="B28" s="30" t="s">
         <v>77</v>
       </c>
-      <c r="C28" s="36" t="s">
+      <c r="C28" s="31" t="s">
         <v>78</v>
       </c>
       <c r="D28" s="17" t="s">
@@ -2954,8 +2962,8 @@
       <c r="A29" s="16" t="s">
         <v>79</v>
       </c>
-      <c r="B29" s="28"/>
-      <c r="C29" s="28"/>
+      <c r="B29" s="29"/>
+      <c r="C29" s="29"/>
       <c r="D29" s="20" t="s">
         <v>43</v>
       </c>
@@ -3012,8 +3020,8 @@
       <c r="A30" s="16" t="s">
         <v>80</v>
       </c>
-      <c r="B30" s="28"/>
-      <c r="C30" s="28"/>
+      <c r="B30" s="29"/>
+      <c r="C30" s="29"/>
       <c r="D30" s="17" t="s">
         <v>48</v>
       </c>
@@ -3070,10 +3078,10 @@
       <c r="A31" s="16" t="s">
         <v>81</v>
       </c>
-      <c r="B31" s="35" t="s">
+      <c r="B31" s="30" t="s">
         <v>82</v>
       </c>
-      <c r="C31" s="36" t="s">
+      <c r="C31" s="31" t="s">
         <v>83</v>
       </c>
       <c r="D31" s="17" t="s">
@@ -3088,27 +3096,41 @@
         <f t="shared" si="0"/>
         <v>26</v>
       </c>
-      <c r="H31" s="37" t="s">
-        <v>101</v>
-      </c>
-      <c r="I31" s="19"/>
-      <c r="J31" s="19"/>
-      <c r="K31" s="19"/>
-      <c r="L31" s="19"/>
-      <c r="M31" s="19"/>
-      <c r="N31" s="19"/>
-      <c r="O31" s="19"/>
+      <c r="H31" s="27" t="s">
+        <v>101</v>
+      </c>
+      <c r="I31" s="27" t="s">
+        <v>115</v>
+      </c>
+      <c r="J31" s="27" t="s">
+        <v>101</v>
+      </c>
+      <c r="K31" s="27" t="s">
+        <v>101</v>
+      </c>
+      <c r="L31" s="27" t="s">
+        <v>101</v>
+      </c>
+      <c r="M31" s="27" t="s">
+        <v>102</v>
+      </c>
+      <c r="N31" s="27" t="s">
+        <v>101</v>
+      </c>
+      <c r="O31" s="27" t="s">
+        <v>116</v>
+      </c>
       <c r="P31" s="11" t="str">
         <f t="shared" si="1"/>
-        <v>0000</v>
+        <v>0004</v>
       </c>
       <c r="Q31" s="12" t="str">
         <f t="shared" si="2"/>
-        <v>0000000000000000</v>
+        <v>0000000000000100</v>
       </c>
       <c r="R31" s="12" t="str">
         <f t="shared" si="3"/>
-        <v>00000000</v>
+        <v>00000100</v>
       </c>
       <c r="S31" s="12" t="str">
         <f t="shared" si="4"/>
@@ -3116,7 +3138,7 @@
       </c>
       <c r="T31" s="12" t="str">
         <f t="shared" ref="T31:U31" si="32">BIN2HEX(R31,2)</f>
-        <v>00</v>
+        <v>04</v>
       </c>
       <c r="U31" s="13" t="str">
         <f t="shared" si="32"/>
@@ -3134,8 +3156,8 @@
       <c r="A32" s="16" t="s">
         <v>84</v>
       </c>
-      <c r="B32" s="28"/>
-      <c r="C32" s="28"/>
+      <c r="B32" s="29"/>
+      <c r="C32" s="29"/>
       <c r="D32" s="20" t="s">
         <v>43</v>
       </c>
@@ -3148,27 +3170,41 @@
         <f t="shared" si="0"/>
         <v>27</v>
       </c>
-      <c r="H32" s="37" t="s">
-        <v>101</v>
-      </c>
-      <c r="I32" s="19"/>
-      <c r="J32" s="19"/>
-      <c r="K32" s="19"/>
-      <c r="L32" s="19"/>
-      <c r="M32" s="19"/>
-      <c r="N32" s="19"/>
-      <c r="O32" s="19"/>
+      <c r="H32" s="27" t="s">
+        <v>101</v>
+      </c>
+      <c r="I32" s="27" t="s">
+        <v>115</v>
+      </c>
+      <c r="J32" s="27" t="s">
+        <v>101</v>
+      </c>
+      <c r="K32" s="27" t="s">
+        <v>101</v>
+      </c>
+      <c r="L32" s="27" t="s">
+        <v>101</v>
+      </c>
+      <c r="M32" s="27" t="s">
+        <v>102</v>
+      </c>
+      <c r="N32" s="27" t="s">
+        <v>101</v>
+      </c>
+      <c r="O32" s="27" t="s">
+        <v>116</v>
+      </c>
       <c r="P32" s="11" t="str">
         <f t="shared" si="1"/>
-        <v>0000</v>
+        <v>0004</v>
       </c>
       <c r="Q32" s="12" t="str">
         <f t="shared" si="2"/>
-        <v>0000000000000000</v>
+        <v>0000000000000100</v>
       </c>
       <c r="R32" s="12" t="str">
         <f t="shared" si="3"/>
-        <v>00000000</v>
+        <v>00000100</v>
       </c>
       <c r="S32" s="12" t="str">
         <f t="shared" si="4"/>
@@ -3176,7 +3212,7 @@
       </c>
       <c r="T32" s="12" t="str">
         <f t="shared" ref="T32:U32" si="33">BIN2HEX(R32,2)</f>
-        <v>00</v>
+        <v>04</v>
       </c>
       <c r="U32" s="13" t="str">
         <f t="shared" si="33"/>
@@ -3194,8 +3230,8 @@
       <c r="A33" s="16" t="s">
         <v>85</v>
       </c>
-      <c r="B33" s="28"/>
-      <c r="C33" s="28"/>
+      <c r="B33" s="29"/>
+      <c r="C33" s="29"/>
       <c r="D33" s="20" t="s">
         <v>50</v>
       </c>
@@ -3208,27 +3244,41 @@
         <f t="shared" si="0"/>
         <v>28</v>
       </c>
-      <c r="H33" s="37" t="s">
-        <v>101</v>
-      </c>
-      <c r="I33" s="19"/>
-      <c r="J33" s="19"/>
-      <c r="K33" s="19"/>
-      <c r="L33" s="19"/>
-      <c r="M33" s="19"/>
-      <c r="N33" s="19"/>
-      <c r="O33" s="19"/>
+      <c r="H33" s="27" t="s">
+        <v>101</v>
+      </c>
+      <c r="I33" s="27" t="s">
+        <v>115</v>
+      </c>
+      <c r="J33" s="27" t="s">
+        <v>101</v>
+      </c>
+      <c r="K33" s="27" t="s">
+        <v>101</v>
+      </c>
+      <c r="L33" s="27" t="s">
+        <v>101</v>
+      </c>
+      <c r="M33" s="27" t="s">
+        <v>102</v>
+      </c>
+      <c r="N33" s="27" t="s">
+        <v>101</v>
+      </c>
+      <c r="O33" s="27" t="s">
+        <v>116</v>
+      </c>
       <c r="P33" s="11" t="str">
         <f t="shared" si="1"/>
-        <v>0000</v>
+        <v>0004</v>
       </c>
       <c r="Q33" s="12" t="str">
         <f t="shared" si="2"/>
-        <v>0000000000000000</v>
+        <v>0000000000000100</v>
       </c>
       <c r="R33" s="12" t="str">
         <f t="shared" si="3"/>
-        <v>00000000</v>
+        <v>00000100</v>
       </c>
       <c r="S33" s="12" t="str">
         <f t="shared" si="4"/>
@@ -3236,7 +3286,7 @@
       </c>
       <c r="T33" s="12" t="str">
         <f t="shared" ref="T33:U33" si="34">BIN2HEX(R33,2)</f>
-        <v>00</v>
+        <v>04</v>
       </c>
       <c r="U33" s="13" t="str">
         <f t="shared" si="34"/>
@@ -3254,8 +3304,8 @@
       <c r="A34" s="16" t="s">
         <v>86</v>
       </c>
-      <c r="B34" s="28"/>
-      <c r="C34" s="28"/>
+      <c r="B34" s="29"/>
+      <c r="C34" s="29"/>
       <c r="D34" s="17" t="s">
         <v>52</v>
       </c>
@@ -3268,27 +3318,41 @@
         <f t="shared" si="0"/>
         <v>29</v>
       </c>
-      <c r="H34" s="37" t="s">
-        <v>101</v>
-      </c>
-      <c r="I34" s="19"/>
-      <c r="J34" s="19"/>
-      <c r="K34" s="19"/>
-      <c r="L34" s="19"/>
-      <c r="M34" s="19"/>
-      <c r="N34" s="19"/>
-      <c r="O34" s="19"/>
+      <c r="H34" s="27" t="s">
+        <v>101</v>
+      </c>
+      <c r="I34" s="27" t="s">
+        <v>115</v>
+      </c>
+      <c r="J34" s="27" t="s">
+        <v>101</v>
+      </c>
+      <c r="K34" s="27" t="s">
+        <v>101</v>
+      </c>
+      <c r="L34" s="27" t="s">
+        <v>101</v>
+      </c>
+      <c r="M34" s="27" t="s">
+        <v>102</v>
+      </c>
+      <c r="N34" s="27" t="s">
+        <v>101</v>
+      </c>
+      <c r="O34" s="27" t="s">
+        <v>116</v>
+      </c>
       <c r="P34" s="11" t="str">
         <f t="shared" si="1"/>
-        <v>0000</v>
+        <v>0004</v>
       </c>
       <c r="Q34" s="12" t="str">
         <f t="shared" si="2"/>
-        <v>0000000000000000</v>
+        <v>0000000000000100</v>
       </c>
       <c r="R34" s="12" t="str">
         <f t="shared" si="3"/>
-        <v>00000000</v>
+        <v>00000100</v>
       </c>
       <c r="S34" s="12" t="str">
         <f t="shared" si="4"/>
@@ -3296,7 +3360,7 @@
       </c>
       <c r="T34" s="12" t="str">
         <f t="shared" ref="T34:U34" si="35">BIN2HEX(R34,2)</f>
-        <v>00</v>
+        <v>04</v>
       </c>
       <c r="U34" s="13" t="str">
         <f t="shared" si="35"/>
@@ -3314,8 +3378,8 @@
       <c r="A35" s="16" t="s">
         <v>87</v>
       </c>
-      <c r="B35" s="28"/>
-      <c r="C35" s="28"/>
+      <c r="B35" s="29"/>
+      <c r="C35" s="29"/>
       <c r="D35" s="17" t="s">
         <v>55</v>
       </c>
@@ -3328,27 +3392,41 @@
         <f t="shared" si="0"/>
         <v>30</v>
       </c>
-      <c r="H35" s="37" t="s">
-        <v>101</v>
-      </c>
-      <c r="I35" s="19"/>
-      <c r="J35" s="19"/>
-      <c r="K35" s="19"/>
-      <c r="L35" s="19"/>
-      <c r="M35" s="19"/>
-      <c r="N35" s="19"/>
-      <c r="O35" s="19"/>
+      <c r="H35" s="27" t="s">
+        <v>101</v>
+      </c>
+      <c r="I35" s="27" t="s">
+        <v>115</v>
+      </c>
+      <c r="J35" s="27" t="s">
+        <v>99</v>
+      </c>
+      <c r="K35" s="27" t="s">
+        <v>101</v>
+      </c>
+      <c r="L35" s="27" t="s">
+        <v>101</v>
+      </c>
+      <c r="M35" s="27" t="s">
+        <v>102</v>
+      </c>
+      <c r="N35" s="27" t="s">
+        <v>101</v>
+      </c>
+      <c r="O35" s="27" t="s">
+        <v>116</v>
+      </c>
       <c r="P35" s="11" t="str">
         <f t="shared" si="1"/>
-        <v>0000</v>
+        <v>0014</v>
       </c>
       <c r="Q35" s="12" t="str">
         <f t="shared" si="2"/>
-        <v>0000000000000000</v>
+        <v>0000000000010100</v>
       </c>
       <c r="R35" s="12" t="str">
         <f t="shared" si="3"/>
-        <v>00000000</v>
+        <v>00010100</v>
       </c>
       <c r="S35" s="12" t="str">
         <f t="shared" si="4"/>
@@ -3356,7 +3434,7 @@
       </c>
       <c r="T35" s="12" t="str">
         <f t="shared" ref="T35:U35" si="36">BIN2HEX(R35,2)</f>
-        <v>00</v>
+        <v>14</v>
       </c>
       <c r="U35" s="13" t="str">
         <f t="shared" si="36"/>
@@ -3374,8 +3452,8 @@
       <c r="A36" s="16" t="s">
         <v>88</v>
       </c>
-      <c r="B36" s="28"/>
-      <c r="C36" s="28"/>
+      <c r="B36" s="29"/>
+      <c r="C36" s="29"/>
       <c r="D36" s="17" t="s">
         <v>57</v>
       </c>
@@ -3388,27 +3466,41 @@
         <f t="shared" si="0"/>
         <v>31</v>
       </c>
-      <c r="H36" s="37" t="s">
-        <v>101</v>
-      </c>
-      <c r="I36" s="19"/>
-      <c r="J36" s="19"/>
-      <c r="K36" s="19"/>
-      <c r="L36" s="19"/>
-      <c r="M36" s="19"/>
-      <c r="N36" s="19"/>
-      <c r="O36" s="19"/>
+      <c r="H36" s="27" t="s">
+        <v>101</v>
+      </c>
+      <c r="I36" s="27" t="s">
+        <v>115</v>
+      </c>
+      <c r="J36" s="27" t="s">
+        <v>99</v>
+      </c>
+      <c r="K36" s="27" t="s">
+        <v>101</v>
+      </c>
+      <c r="L36" s="27" t="s">
+        <v>101</v>
+      </c>
+      <c r="M36" s="27" t="s">
+        <v>102</v>
+      </c>
+      <c r="N36" s="27" t="s">
+        <v>101</v>
+      </c>
+      <c r="O36" s="27" t="s">
+        <v>116</v>
+      </c>
       <c r="P36" s="11" t="str">
         <f t="shared" si="1"/>
-        <v>0000</v>
+        <v>0014</v>
       </c>
       <c r="Q36" s="12" t="str">
         <f t="shared" si="2"/>
-        <v>0000000000000000</v>
+        <v>0000000000010100</v>
       </c>
       <c r="R36" s="12" t="str">
         <f t="shared" si="3"/>
-        <v>00000000</v>
+        <v>00010100</v>
       </c>
       <c r="S36" s="12" t="str">
         <f t="shared" si="4"/>
@@ -3416,7 +3508,7 @@
       </c>
       <c r="T36" s="12" t="str">
         <f t="shared" ref="T36:U36" si="37">BIN2HEX(R36,2)</f>
-        <v>00</v>
+        <v>14</v>
       </c>
       <c r="U36" s="13" t="str">
         <f t="shared" si="37"/>
@@ -3434,7 +3526,7 @@
       <c r="A37" s="16" t="s">
         <v>89</v>
       </c>
-      <c r="B37" s="35" t="s">
+      <c r="B37" s="30" t="s">
         <v>90</v>
       </c>
       <c r="C37" s="25" t="s">
@@ -3494,7 +3586,7 @@
       <c r="A38" s="16" t="s">
         <v>92</v>
       </c>
-      <c r="B38" s="28"/>
+      <c r="B38" s="29"/>
       <c r="C38" s="25" t="s">
         <v>93</v>
       </c>
@@ -3672,6 +3764,12 @@
     </row>
   </sheetData>
   <mergeCells count="16">
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="B1:E1"/>
+    <mergeCell ref="F1:G1"/>
+    <mergeCell ref="H1:O1"/>
+    <mergeCell ref="Q1:W1"/>
+    <mergeCell ref="H2:O2"/>
     <mergeCell ref="C5:C16"/>
     <mergeCell ref="B31:B36"/>
     <mergeCell ref="B37:B38"/>
@@ -3682,12 +3780,6 @@
     <mergeCell ref="B28:B30"/>
     <mergeCell ref="C28:C30"/>
     <mergeCell ref="C31:C36"/>
-    <mergeCell ref="A1:A2"/>
-    <mergeCell ref="B1:E1"/>
-    <mergeCell ref="F1:G1"/>
-    <mergeCell ref="H1:O1"/>
-    <mergeCell ref="Q1:W1"/>
-    <mergeCell ref="H2:O2"/>
   </mergeCells>
   <phoneticPr fontId="13" type="noConversion"/>
   <conditionalFormatting sqref="A1:A2">

</xml_diff>

<commit_message>
done proj3, well, I made a cpu
</commit_message>
<xml_diff>
--- a/61c-proj3/fa24-proj3-starter/[61C FA24] Project 3B ROM Control Logic.xlsx
+++ b/61c-proj3/fa24-proj3-starter/[61C FA24] Project 3B ROM Control Logic.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Courses\UCB CS61C 2024Fall\61c-proj3\fa24-proj3-starter\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{736673C7-30B7-4E91-9113-59ED4F355C49}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14AC6D2F-AFBB-43E4-A543-DB9EB41EA9B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14295" yWindow="0" windowWidth="14610" windowHeight="15585" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="8535" yWindow="0" windowWidth="13148" windowHeight="12863" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Control Logic for ROM" sheetId="1" r:id="rId1"/>
@@ -145,7 +145,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="346" uniqueCount="117">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="426" uniqueCount="122">
   <si>
     <t>MAKE A COPY OF THIS SHEET</t>
   </si>
@@ -513,6 +513,26 @@
   </si>
   <si>
     <t>00</t>
+    <phoneticPr fontId="13" type="noConversion"/>
+  </si>
+  <si>
+    <t>001</t>
+    <phoneticPr fontId="13" type="noConversion"/>
+  </si>
+  <si>
+    <t>100</t>
+    <phoneticPr fontId="13" type="noConversion"/>
+  </si>
+  <si>
+    <t>10</t>
+    <phoneticPr fontId="13" type="noConversion"/>
+  </si>
+  <si>
+    <t>1111</t>
+    <phoneticPr fontId="13" type="noConversion"/>
+  </si>
+  <si>
+    <t>011</t>
     <phoneticPr fontId="13" type="noConversion"/>
   </si>
 </sst>
@@ -751,19 +771,10 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -776,6 +787,15 @@
     </xf>
     <xf numFmtId="49" fontId="4" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1007,40 +1027,40 @@
   <dimension ref="A1:W40"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="4" topLeftCell="H13" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="4" topLeftCell="I21" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="P5" sqref="P5:P40"/>
+      <selection pane="bottomRight" activeCell="O38" sqref="O38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="12.59765625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="15.7109375" customWidth="1"/>
-    <col min="2" max="2" width="5.42578125" customWidth="1"/>
-    <col min="3" max="3" width="9.85546875" customWidth="1"/>
-    <col min="4" max="4" width="7.42578125" customWidth="1"/>
-    <col min="5" max="5" width="11.42578125" customWidth="1"/>
-    <col min="6" max="6" width="10.28515625" customWidth="1"/>
+    <col min="1" max="1" width="15.73046875" customWidth="1"/>
+    <col min="2" max="2" width="5.3984375" customWidth="1"/>
+    <col min="3" max="3" width="9.86328125" customWidth="1"/>
+    <col min="4" max="4" width="7.3984375" customWidth="1"/>
+    <col min="5" max="5" width="11.3984375" customWidth="1"/>
+    <col min="6" max="6" width="10.265625" customWidth="1"/>
     <col min="7" max="7" width="7" customWidth="1"/>
-    <col min="17" max="17" width="16.7109375" hidden="1" customWidth="1"/>
-    <col min="18" max="23" width="12.5703125" hidden="1"/>
+    <col min="17" max="17" width="16.73046875" hidden="1" customWidth="1"/>
+    <col min="18" max="23" width="12.59765625" hidden="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="32" t="s">
+    <row r="1" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A1" s="28" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="33" t="s">
+      <c r="B1" s="30" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="29"/>
       <c r="D1" s="29"/>
-      <c r="E1" s="34"/>
-      <c r="F1" s="33" t="s">
+      <c r="E1" s="31"/>
+      <c r="F1" s="30" t="s">
         <v>2</v>
       </c>
-      <c r="G1" s="34"/>
-      <c r="H1" s="35" t="s">
+      <c r="G1" s="31"/>
+      <c r="H1" s="32" t="s">
         <v>3</v>
       </c>
       <c r="I1" s="29"/>
@@ -1049,11 +1069,11 @@
       <c r="L1" s="29"/>
       <c r="M1" s="29"/>
       <c r="N1" s="29"/>
-      <c r="O1" s="34"/>
+      <c r="O1" s="31"/>
       <c r="P1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="Q1" s="36" t="s">
+      <c r="Q1" s="33" t="s">
         <v>5</v>
       </c>
       <c r="R1" s="29"/>
@@ -1063,7 +1083,7 @@
       <c r="V1" s="29"/>
       <c r="W1" s="29"/>
     </row>
-    <row r="2" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A2" s="29"/>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
@@ -1071,7 +1091,7 @@
       <c r="E2" s="4"/>
       <c r="F2" s="1"/>
       <c r="G2" s="4"/>
-      <c r="H2" s="37" t="s">
+      <c r="H2" s="34" t="s">
         <v>6</v>
       </c>
       <c r="I2" s="29"/>
@@ -1080,7 +1100,7 @@
       <c r="L2" s="29"/>
       <c r="M2" s="29"/>
       <c r="N2" s="29"/>
-      <c r="O2" s="34"/>
+      <c r="O2" s="31"/>
       <c r="P2" s="2"/>
       <c r="Q2" s="3"/>
       <c r="R2" s="3"/>
@@ -1090,7 +1110,7 @@
       <c r="V2" s="3"/>
       <c r="W2" s="3"/>
     </row>
-    <row r="3" spans="1:23" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:23" ht="13.15" x14ac:dyDescent="0.4">
       <c r="A3" s="5" t="s">
         <v>7</v>
       </c>
@@ -1161,7 +1181,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="4" spans="1:23" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:23" ht="13.15" x14ac:dyDescent="0.35">
       <c r="A4" s="5"/>
       <c r="B4" s="6"/>
       <c r="C4" s="6"/>
@@ -1202,14 +1222,14 @@
       <c r="V4" s="12"/>
       <c r="W4" s="12"/>
     </row>
-    <row r="5" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A5" s="16" t="s">
         <v>33</v>
       </c>
-      <c r="B5" s="30" t="s">
+      <c r="B5" s="36" t="s">
         <v>34</v>
       </c>
-      <c r="C5" s="28" t="s">
+      <c r="C5" s="35" t="s">
         <v>35</v>
       </c>
       <c r="D5" s="17" t="s">
@@ -1282,7 +1302,7 @@
         <v>000000</v>
       </c>
     </row>
-    <row r="6" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A6" s="16" t="s">
         <v>38</v>
       </c>
@@ -1358,7 +1378,7 @@
         <v>000001</v>
       </c>
     </row>
-    <row r="7" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A7" s="16" t="s">
         <v>40</v>
       </c>
@@ -1434,7 +1454,7 @@
         <v>000010</v>
       </c>
     </row>
-    <row r="8" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A8" s="16" t="s">
         <v>42</v>
       </c>
@@ -1510,7 +1530,7 @@
         <v>000011</v>
       </c>
     </row>
-    <row r="9" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A9" s="16" t="s">
         <v>44</v>
       </c>
@@ -1586,7 +1606,7 @@
         <v>000100</v>
       </c>
     </row>
-    <row r="10" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A10" s="16" t="s">
         <v>45</v>
       </c>
@@ -1662,7 +1682,7 @@
         <v>000101</v>
       </c>
     </row>
-    <row r="11" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A11" s="16" t="s">
         <v>47</v>
       </c>
@@ -1738,7 +1758,7 @@
         <v>000110</v>
       </c>
     </row>
-    <row r="12" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A12" s="16" t="s">
         <v>49</v>
       </c>
@@ -1814,7 +1834,7 @@
         <v>000111</v>
       </c>
     </row>
-    <row r="13" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A13" s="16" t="s">
         <v>51</v>
       </c>
@@ -1890,7 +1910,7 @@
         <v>001000</v>
       </c>
     </row>
-    <row r="14" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A14" s="16" t="s">
         <v>53</v>
       </c>
@@ -1966,7 +1986,7 @@
         <v>001001</v>
       </c>
     </row>
-    <row r="15" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A15" s="16" t="s">
         <v>54</v>
       </c>
@@ -2042,7 +2062,7 @@
         <v>001010</v>
       </c>
     </row>
-    <row r="16" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A16" s="16" t="s">
         <v>56</v>
       </c>
@@ -2118,14 +2138,14 @@
         <v>001011</v>
       </c>
     </row>
-    <row r="17" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A17" s="16" t="s">
         <v>58</v>
       </c>
-      <c r="B17" s="30" t="s">
+      <c r="B17" s="36" t="s">
         <v>59</v>
       </c>
-      <c r="C17" s="31" t="s">
+      <c r="C17" s="37" t="s">
         <v>60</v>
       </c>
       <c r="D17" s="17" t="s">
@@ -2140,33 +2160,49 @@
         <f t="shared" si="0"/>
         <v>12</v>
       </c>
-      <c r="H17" s="19"/>
-      <c r="I17" s="19"/>
-      <c r="J17" s="19"/>
-      <c r="K17" s="19"/>
-      <c r="L17" s="19"/>
-      <c r="M17" s="19"/>
-      <c r="N17" s="19"/>
-      <c r="O17" s="19"/>
+      <c r="H17" s="27" t="s">
+        <v>99</v>
+      </c>
+      <c r="I17" s="27" t="s">
+        <v>100</v>
+      </c>
+      <c r="J17" s="27" t="s">
+        <v>101</v>
+      </c>
+      <c r="K17" s="27" t="s">
+        <v>99</v>
+      </c>
+      <c r="L17" s="27" t="s">
+        <v>101</v>
+      </c>
+      <c r="M17" s="27" t="s">
+        <v>102</v>
+      </c>
+      <c r="N17" s="27" t="s">
+        <v>101</v>
+      </c>
+      <c r="O17" s="27" t="s">
+        <v>116</v>
+      </c>
       <c r="P17" s="11" t="str">
         <f t="shared" si="1"/>
-        <v>0000</v>
+        <v>0021</v>
       </c>
       <c r="Q17" s="12" t="str">
         <f t="shared" si="2"/>
-        <v/>
+        <v>0000000000100001</v>
       </c>
       <c r="R17" s="12" t="str">
         <f t="shared" si="3"/>
-        <v/>
+        <v>00100001</v>
       </c>
       <c r="S17" s="12" t="str">
         <f t="shared" si="4"/>
-        <v/>
+        <v>00000000</v>
       </c>
       <c r="T17" s="12" t="str">
         <f t="shared" ref="T17:U17" si="18">BIN2HEX(R17,2)</f>
-        <v>00</v>
+        <v>21</v>
       </c>
       <c r="U17" s="13" t="str">
         <f t="shared" si="18"/>
@@ -2180,7 +2216,7 @@
         <v>001100</v>
       </c>
     </row>
-    <row r="18" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A18" s="16" t="s">
         <v>61</v>
       </c>
@@ -2198,33 +2234,49 @@
         <f t="shared" si="0"/>
         <v>13</v>
       </c>
-      <c r="H18" s="19"/>
-      <c r="I18" s="19"/>
-      <c r="J18" s="19"/>
-      <c r="K18" s="19"/>
-      <c r="L18" s="19"/>
-      <c r="M18" s="19"/>
-      <c r="N18" s="19"/>
-      <c r="O18" s="19"/>
+      <c r="H18" s="27" t="s">
+        <v>99</v>
+      </c>
+      <c r="I18" s="27" t="s">
+        <v>100</v>
+      </c>
+      <c r="J18" s="27" t="s">
+        <v>101</v>
+      </c>
+      <c r="K18" s="27" t="s">
+        <v>99</v>
+      </c>
+      <c r="L18" s="27" t="s">
+        <v>101</v>
+      </c>
+      <c r="M18" s="27" t="s">
+        <v>102</v>
+      </c>
+      <c r="N18" s="27" t="s">
+        <v>101</v>
+      </c>
+      <c r="O18" s="27" t="s">
+        <v>116</v>
+      </c>
       <c r="P18" s="11" t="str">
         <f t="shared" si="1"/>
-        <v>0000</v>
+        <v>0021</v>
       </c>
       <c r="Q18" s="12" t="str">
         <f t="shared" si="2"/>
-        <v/>
+        <v>0000000000100001</v>
       </c>
       <c r="R18" s="12" t="str">
         <f t="shared" si="3"/>
-        <v/>
+        <v>00100001</v>
       </c>
       <c r="S18" s="12" t="str">
         <f t="shared" si="4"/>
-        <v/>
+        <v>00000000</v>
       </c>
       <c r="T18" s="12" t="str">
         <f t="shared" ref="T18:U18" si="19">BIN2HEX(R18,2)</f>
-        <v>00</v>
+        <v>21</v>
       </c>
       <c r="U18" s="13" t="str">
         <f t="shared" si="19"/>
@@ -2238,7 +2290,7 @@
         <v>001101</v>
       </c>
     </row>
-    <row r="19" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A19" s="16" t="s">
         <v>62</v>
       </c>
@@ -2256,33 +2308,49 @@
         <f t="shared" si="0"/>
         <v>14</v>
       </c>
-      <c r="H19" s="19"/>
-      <c r="I19" s="19"/>
-      <c r="J19" s="19"/>
-      <c r="K19" s="19"/>
-      <c r="L19" s="19"/>
-      <c r="M19" s="19"/>
-      <c r="N19" s="19"/>
-      <c r="O19" s="19"/>
+      <c r="H19" s="27" t="s">
+        <v>99</v>
+      </c>
+      <c r="I19" s="27" t="s">
+        <v>100</v>
+      </c>
+      <c r="J19" s="27" t="s">
+        <v>101</v>
+      </c>
+      <c r="K19" s="27" t="s">
+        <v>99</v>
+      </c>
+      <c r="L19" s="27" t="s">
+        <v>101</v>
+      </c>
+      <c r="M19" s="27" t="s">
+        <v>102</v>
+      </c>
+      <c r="N19" s="27" t="s">
+        <v>101</v>
+      </c>
+      <c r="O19" s="27" t="s">
+        <v>116</v>
+      </c>
       <c r="P19" s="11" t="str">
         <f t="shared" si="1"/>
-        <v>0000</v>
+        <v>0021</v>
       </c>
       <c r="Q19" s="12" t="str">
         <f t="shared" si="2"/>
-        <v/>
+        <v>0000000000100001</v>
       </c>
       <c r="R19" s="12" t="str">
         <f t="shared" si="3"/>
-        <v/>
+        <v>00100001</v>
       </c>
       <c r="S19" s="12" t="str">
         <f t="shared" si="4"/>
-        <v/>
+        <v>00000000</v>
       </c>
       <c r="T19" s="12" t="str">
         <f t="shared" ref="T19:U19" si="20">BIN2HEX(R19,2)</f>
-        <v>00</v>
+        <v>21</v>
       </c>
       <c r="U19" s="13" t="str">
         <f t="shared" si="20"/>
@@ -2296,12 +2364,12 @@
         <v>001110</v>
       </c>
     </row>
-    <row r="20" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A20" s="16" t="s">
         <v>63</v>
       </c>
       <c r="B20" s="29"/>
-      <c r="C20" s="31" t="s">
+      <c r="C20" s="37" t="s">
         <v>64</v>
       </c>
       <c r="D20" s="17" t="s">
@@ -2372,7 +2440,7 @@
         <v>001111</v>
       </c>
     </row>
-    <row r="21" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A21" s="16" t="s">
         <v>69</v>
       </c>
@@ -2448,7 +2516,7 @@
         <v>010000</v>
       </c>
     </row>
-    <row r="22" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A22" s="16" t="s">
         <v>70</v>
       </c>
@@ -2522,7 +2590,7 @@
         <v>010001</v>
       </c>
     </row>
-    <row r="23" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A23" s="16" t="s">
         <v>71</v>
       </c>
@@ -2596,7 +2664,7 @@
         <v>010010</v>
       </c>
     </row>
-    <row r="24" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A24" s="16" t="s">
         <v>72</v>
       </c>
@@ -2672,7 +2740,7 @@
         <v>010011</v>
       </c>
     </row>
-    <row r="25" spans="1:23" ht="13.5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:23" ht="13.5" x14ac:dyDescent="0.45">
       <c r="A25" s="16" t="s">
         <v>73</v>
       </c>
@@ -2748,7 +2816,7 @@
         <v>010100</v>
       </c>
     </row>
-    <row r="26" spans="1:23" ht="13.5" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:23" ht="13.5" x14ac:dyDescent="0.45">
       <c r="A26" s="16" t="s">
         <v>74</v>
       </c>
@@ -2822,7 +2890,7 @@
         <v>010101</v>
       </c>
     </row>
-    <row r="27" spans="1:23" ht="13.5" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:23" ht="13.5" x14ac:dyDescent="0.45">
       <c r="A27" s="16" t="s">
         <v>75</v>
       </c>
@@ -2896,14 +2964,14 @@
         <v>010110</v>
       </c>
     </row>
-    <row r="28" spans="1:23" ht="13.5" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:23" ht="13.5" x14ac:dyDescent="0.45">
       <c r="A28" s="16" t="s">
         <v>76</v>
       </c>
-      <c r="B28" s="30" t="s">
+      <c r="B28" s="36" t="s">
         <v>77</v>
       </c>
-      <c r="C28" s="31" t="s">
+      <c r="C28" s="37" t="s">
         <v>78</v>
       </c>
       <c r="D28" s="17" t="s">
@@ -2918,37 +2986,53 @@
         <f t="shared" si="0"/>
         <v>23</v>
       </c>
-      <c r="H28" s="19"/>
-      <c r="I28" s="19"/>
-      <c r="J28" s="19"/>
-      <c r="K28" s="19"/>
-      <c r="L28" s="19"/>
-      <c r="M28" s="19"/>
-      <c r="N28" s="19"/>
-      <c r="O28" s="19"/>
+      <c r="H28" s="27" t="s">
+        <v>101</v>
+      </c>
+      <c r="I28" s="27" t="s">
+        <v>117</v>
+      </c>
+      <c r="J28" s="27" t="s">
+        <v>101</v>
+      </c>
+      <c r="K28" s="27" t="s">
+        <v>99</v>
+      </c>
+      <c r="L28" s="27" t="s">
+        <v>101</v>
+      </c>
+      <c r="M28" s="27" t="s">
+        <v>102</v>
+      </c>
+      <c r="N28" s="27" t="s">
+        <v>99</v>
+      </c>
+      <c r="O28" s="27" t="s">
+        <v>116</v>
+      </c>
       <c r="P28" s="11" t="str">
         <f t="shared" si="1"/>
-        <v>0000</v>
+        <v>0822</v>
       </c>
       <c r="Q28" s="12" t="str">
         <f t="shared" si="2"/>
-        <v/>
+        <v>0000100000100010</v>
       </c>
       <c r="R28" s="12" t="str">
         <f t="shared" si="3"/>
-        <v/>
+        <v>00100010</v>
       </c>
       <c r="S28" s="12" t="str">
         <f t="shared" si="4"/>
-        <v/>
+        <v>00001000</v>
       </c>
       <c r="T28" s="12" t="str">
         <f t="shared" ref="T28:U28" si="29">BIN2HEX(R28,2)</f>
-        <v>00</v>
+        <v>22</v>
       </c>
       <c r="U28" s="13" t="str">
         <f t="shared" si="29"/>
-        <v>00</v>
+        <v>08</v>
       </c>
       <c r="V28" s="12">
         <v>23</v>
@@ -2958,7 +3042,7 @@
         <v>010111</v>
       </c>
     </row>
-    <row r="29" spans="1:23" ht="13.5" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:23" ht="13.5" x14ac:dyDescent="0.45">
       <c r="A29" s="16" t="s">
         <v>79</v>
       </c>
@@ -2976,37 +3060,53 @@
         <f t="shared" si="0"/>
         <v>24</v>
       </c>
-      <c r="H29" s="19"/>
-      <c r="I29" s="19"/>
-      <c r="J29" s="19"/>
-      <c r="K29" s="19"/>
-      <c r="L29" s="19"/>
-      <c r="M29" s="19"/>
-      <c r="N29" s="19"/>
-      <c r="O29" s="19"/>
+      <c r="H29" s="27" t="s">
+        <v>101</v>
+      </c>
+      <c r="I29" s="27" t="s">
+        <v>117</v>
+      </c>
+      <c r="J29" s="27" t="s">
+        <v>101</v>
+      </c>
+      <c r="K29" s="27" t="s">
+        <v>99</v>
+      </c>
+      <c r="L29" s="27" t="s">
+        <v>101</v>
+      </c>
+      <c r="M29" s="27" t="s">
+        <v>102</v>
+      </c>
+      <c r="N29" s="27" t="s">
+        <v>99</v>
+      </c>
+      <c r="O29" s="27" t="s">
+        <v>116</v>
+      </c>
       <c r="P29" s="11" t="str">
         <f t="shared" si="1"/>
-        <v>0000</v>
+        <v>0822</v>
       </c>
       <c r="Q29" s="12" t="str">
         <f t="shared" si="2"/>
-        <v/>
+        <v>0000100000100010</v>
       </c>
       <c r="R29" s="12" t="str">
         <f t="shared" si="3"/>
-        <v/>
+        <v>00100010</v>
       </c>
       <c r="S29" s="12" t="str">
         <f t="shared" si="4"/>
-        <v/>
+        <v>00001000</v>
       </c>
       <c r="T29" s="12" t="str">
         <f t="shared" ref="T29:U29" si="30">BIN2HEX(R29,2)</f>
-        <v>00</v>
+        <v>22</v>
       </c>
       <c r="U29" s="13" t="str">
         <f t="shared" si="30"/>
-        <v>00</v>
+        <v>08</v>
       </c>
       <c r="V29" s="12">
         <v>24</v>
@@ -3016,7 +3116,7 @@
         <v>011000</v>
       </c>
     </row>
-    <row r="30" spans="1:23" ht="13.5" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:23" ht="13.5" x14ac:dyDescent="0.45">
       <c r="A30" s="16" t="s">
         <v>80</v>
       </c>
@@ -3034,37 +3134,53 @@
         <f t="shared" si="0"/>
         <v>25</v>
       </c>
-      <c r="H30" s="19"/>
-      <c r="I30" s="19"/>
-      <c r="J30" s="19"/>
-      <c r="K30" s="19"/>
-      <c r="L30" s="19"/>
-      <c r="M30" s="19"/>
-      <c r="N30" s="19"/>
-      <c r="O30" s="19"/>
+      <c r="H30" s="27" t="s">
+        <v>101</v>
+      </c>
+      <c r="I30" s="27" t="s">
+        <v>117</v>
+      </c>
+      <c r="J30" s="27" t="s">
+        <v>101</v>
+      </c>
+      <c r="K30" s="27" t="s">
+        <v>99</v>
+      </c>
+      <c r="L30" s="27" t="s">
+        <v>101</v>
+      </c>
+      <c r="M30" s="27" t="s">
+        <v>102</v>
+      </c>
+      <c r="N30" s="27" t="s">
+        <v>99</v>
+      </c>
+      <c r="O30" s="27" t="s">
+        <v>116</v>
+      </c>
       <c r="P30" s="11" t="str">
         <f t="shared" si="1"/>
-        <v>0000</v>
+        <v>0822</v>
       </c>
       <c r="Q30" s="12" t="str">
         <f t="shared" si="2"/>
-        <v/>
+        <v>0000100000100010</v>
       </c>
       <c r="R30" s="12" t="str">
         <f t="shared" si="3"/>
-        <v/>
+        <v>00100010</v>
       </c>
       <c r="S30" s="12" t="str">
         <f t="shared" si="4"/>
-        <v/>
+        <v>00001000</v>
       </c>
       <c r="T30" s="12" t="str">
         <f t="shared" ref="T30:U30" si="31">BIN2HEX(R30,2)</f>
-        <v>00</v>
+        <v>22</v>
       </c>
       <c r="U30" s="13" t="str">
         <f t="shared" si="31"/>
-        <v>00</v>
+        <v>08</v>
       </c>
       <c r="V30" s="12">
         <v>25</v>
@@ -3074,14 +3190,14 @@
         <v>011001</v>
       </c>
     </row>
-    <row r="31" spans="1:23" ht="13.5" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:23" ht="13.5" x14ac:dyDescent="0.45">
       <c r="A31" s="16" t="s">
         <v>81</v>
       </c>
-      <c r="B31" s="30" t="s">
+      <c r="B31" s="36" t="s">
         <v>82</v>
       </c>
-      <c r="C31" s="31" t="s">
+      <c r="C31" s="37" t="s">
         <v>83</v>
       </c>
       <c r="D31" s="17" t="s">
@@ -3152,7 +3268,7 @@
         <v>011010</v>
       </c>
     </row>
-    <row r="32" spans="1:23" ht="13.5" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:23" ht="13.5" x14ac:dyDescent="0.45">
       <c r="A32" s="16" t="s">
         <v>84</v>
       </c>
@@ -3226,7 +3342,7 @@
         <v>011011</v>
       </c>
     </row>
-    <row r="33" spans="1:23" ht="13.5" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:23" ht="13.5" x14ac:dyDescent="0.45">
       <c r="A33" s="16" t="s">
         <v>85</v>
       </c>
@@ -3300,7 +3416,7 @@
         <v>011100</v>
       </c>
     </row>
-    <row r="34" spans="1:23" ht="13.5" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:23" ht="13.5" x14ac:dyDescent="0.45">
       <c r="A34" s="16" t="s">
         <v>86</v>
       </c>
@@ -3374,7 +3490,7 @@
         <v>011101</v>
       </c>
     </row>
-    <row r="35" spans="1:23" ht="13.5" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:23" ht="13.5" x14ac:dyDescent="0.45">
       <c r="A35" s="16" t="s">
         <v>87</v>
       </c>
@@ -3448,7 +3564,7 @@
         <v>011110</v>
       </c>
     </row>
-    <row r="36" spans="1:23" ht="13.5" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:23" ht="13.5" x14ac:dyDescent="0.45">
       <c r="A36" s="16" t="s">
         <v>88</v>
       </c>
@@ -3522,11 +3638,11 @@
         <v>011111</v>
       </c>
     </row>
-    <row r="37" spans="1:23" ht="13.5" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:23" ht="13.5" x14ac:dyDescent="0.45">
       <c r="A37" s="16" t="s">
         <v>89</v>
       </c>
-      <c r="B37" s="30" t="s">
+      <c r="B37" s="36" t="s">
         <v>90</v>
       </c>
       <c r="C37" s="25" t="s">
@@ -3542,37 +3658,53 @@
         <f t="shared" si="0"/>
         <v>32</v>
       </c>
-      <c r="H37" s="19"/>
-      <c r="I37" s="19"/>
-      <c r="J37" s="19"/>
-      <c r="K37" s="19"/>
-      <c r="L37" s="19"/>
-      <c r="M37" s="19"/>
-      <c r="N37" s="19"/>
-      <c r="O37" s="19"/>
+      <c r="H37" s="27" t="s">
+        <v>99</v>
+      </c>
+      <c r="I37" s="27" t="s">
+        <v>121</v>
+      </c>
+      <c r="J37" s="27" t="s">
+        <v>101</v>
+      </c>
+      <c r="K37" s="27" t="s">
+        <v>101</v>
+      </c>
+      <c r="L37" s="27" t="s">
+        <v>101</v>
+      </c>
+      <c r="M37" s="27" t="s">
+        <v>102</v>
+      </c>
+      <c r="N37" s="27" t="s">
+        <v>101</v>
+      </c>
+      <c r="O37" s="27" t="s">
+        <v>114</v>
+      </c>
       <c r="P37" s="11" t="str">
         <f>CONCATENATE(U37,T37)</f>
-        <v>0000</v>
+        <v>1007</v>
       </c>
       <c r="Q37" s="12" t="str">
         <f t="shared" si="2"/>
-        <v/>
+        <v>0001000000000111</v>
       </c>
       <c r="R37" s="12" t="str">
         <f t="shared" si="3"/>
-        <v/>
+        <v>00000111</v>
       </c>
       <c r="S37" s="12" t="str">
         <f t="shared" si="4"/>
-        <v/>
+        <v>00010000</v>
       </c>
       <c r="T37" s="12" t="str">
         <f t="shared" ref="T37:U37" si="38">BIN2HEX(R37,2)</f>
-        <v>00</v>
+        <v>07</v>
       </c>
       <c r="U37" s="13" t="str">
         <f t="shared" si="38"/>
-        <v>00</v>
+        <v>10</v>
       </c>
       <c r="V37" s="12">
         <v>32</v>
@@ -3582,7 +3714,7 @@
         <v>100000</v>
       </c>
     </row>
-    <row r="38" spans="1:23" ht="13.5" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:23" ht="13.5" x14ac:dyDescent="0.45">
       <c r="A38" s="16" t="s">
         <v>92</v>
       </c>
@@ -3600,37 +3732,53 @@
         <f t="shared" si="0"/>
         <v>33</v>
       </c>
-      <c r="H38" s="19"/>
-      <c r="I38" s="19"/>
-      <c r="J38" s="19"/>
-      <c r="K38" s="19"/>
-      <c r="L38" s="19"/>
-      <c r="M38" s="19"/>
-      <c r="N38" s="19"/>
-      <c r="O38" s="19"/>
+      <c r="H38" s="27" t="s">
+        <v>99</v>
+      </c>
+      <c r="I38" s="27" t="s">
+        <v>121</v>
+      </c>
+      <c r="J38" s="27" t="s">
+        <v>101</v>
+      </c>
+      <c r="K38" s="27" t="s">
+        <v>101</v>
+      </c>
+      <c r="L38" s="27" t="s">
+        <v>101</v>
+      </c>
+      <c r="M38" s="27" t="s">
+        <v>120</v>
+      </c>
+      <c r="N38" s="27" t="s">
+        <v>101</v>
+      </c>
+      <c r="O38" s="27" t="s">
+        <v>114</v>
+      </c>
       <c r="P38" s="11" t="str">
         <f t="shared" si="1"/>
-        <v>0000</v>
+        <v>1787</v>
       </c>
       <c r="Q38" s="12" t="str">
         <f t="shared" si="2"/>
-        <v/>
+        <v>0001011110000111</v>
       </c>
       <c r="R38" s="12" t="str">
         <f t="shared" si="3"/>
-        <v/>
+        <v>10000111</v>
       </c>
       <c r="S38" s="12" t="str">
         <f t="shared" si="4"/>
-        <v/>
+        <v>00010111</v>
       </c>
       <c r="T38" s="12" t="str">
         <f t="shared" ref="T38:U38" si="39">BIN2HEX(R38,2)</f>
-        <v>00</v>
+        <v>87</v>
       </c>
       <c r="U38" s="13" t="str">
         <f t="shared" si="39"/>
-        <v>00</v>
+        <v>17</v>
       </c>
       <c r="V38" s="12">
         <v>33</v>
@@ -3640,7 +3788,7 @@
         <v>100001</v>
       </c>
     </row>
-    <row r="39" spans="1:23" ht="13.5" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:23" ht="13.5" x14ac:dyDescent="0.45">
       <c r="A39" s="16" t="s">
         <v>94</v>
       </c>
@@ -3660,37 +3808,53 @@
         <f t="shared" si="0"/>
         <v>34</v>
       </c>
-      <c r="H39" s="19"/>
-      <c r="I39" s="19"/>
-      <c r="J39" s="19"/>
-      <c r="K39" s="19"/>
-      <c r="L39" s="19"/>
-      <c r="M39" s="19"/>
-      <c r="N39" s="19"/>
-      <c r="O39" s="19"/>
+      <c r="H39" s="27" t="s">
+        <v>99</v>
+      </c>
+      <c r="I39" s="27" t="s">
+        <v>118</v>
+      </c>
+      <c r="J39" s="27" t="s">
+        <v>101</v>
+      </c>
+      <c r="K39" s="27" t="s">
+        <v>101</v>
+      </c>
+      <c r="L39" s="27" t="s">
+        <v>101</v>
+      </c>
+      <c r="M39" s="27" t="s">
+        <v>102</v>
+      </c>
+      <c r="N39" s="27" t="s">
+        <v>101</v>
+      </c>
+      <c r="O39" s="27" t="s">
+        <v>119</v>
+      </c>
       <c r="P39" s="11" t="str">
         <f t="shared" si="1"/>
-        <v>0000</v>
+        <v>2009</v>
       </c>
       <c r="Q39" s="12" t="str">
         <f t="shared" si="2"/>
-        <v/>
+        <v>0010000000001001</v>
       </c>
       <c r="R39" s="12" t="str">
         <f t="shared" si="3"/>
-        <v/>
+        <v>00001001</v>
       </c>
       <c r="S39" s="12" t="str">
         <f t="shared" si="4"/>
-        <v/>
+        <v>00100000</v>
       </c>
       <c r="T39" s="12" t="str">
         <f t="shared" ref="T39:U39" si="40">BIN2HEX(R39,2)</f>
-        <v>00</v>
+        <v>09</v>
       </c>
       <c r="U39" s="13" t="str">
         <f t="shared" si="40"/>
-        <v>00</v>
+        <v>20</v>
       </c>
       <c r="V39" s="12">
         <v>34</v>
@@ -3700,7 +3864,7 @@
         <v>100010</v>
       </c>
     </row>
-    <row r="40" spans="1:23" ht="13.5" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:23" ht="13.5" x14ac:dyDescent="0.45">
       <c r="A40" s="16" t="s">
         <v>97</v>
       </c>
@@ -3722,37 +3886,53 @@
         <f t="shared" si="0"/>
         <v>35</v>
       </c>
-      <c r="H40" s="19"/>
-      <c r="I40" s="19"/>
-      <c r="J40" s="19"/>
-      <c r="K40" s="19"/>
-      <c r="L40" s="19"/>
-      <c r="M40" s="19"/>
-      <c r="N40" s="19"/>
-      <c r="O40" s="19"/>
+      <c r="H40" s="27" t="s">
+        <v>99</v>
+      </c>
+      <c r="I40" s="27" t="s">
+        <v>100</v>
+      </c>
+      <c r="J40" s="27" t="s">
+        <v>101</v>
+      </c>
+      <c r="K40" s="27" t="s">
+        <v>99</v>
+      </c>
+      <c r="L40" s="27" t="s">
+        <v>101</v>
+      </c>
+      <c r="M40" s="27" t="s">
+        <v>102</v>
+      </c>
+      <c r="N40" s="27" t="s">
+        <v>101</v>
+      </c>
+      <c r="O40" s="27" t="s">
+        <v>119</v>
+      </c>
       <c r="P40" s="11" t="str">
         <f t="shared" si="1"/>
-        <v>0000</v>
+        <v>2021</v>
       </c>
       <c r="Q40" s="12" t="str">
         <f t="shared" si="2"/>
-        <v/>
+        <v>0010000000100001</v>
       </c>
       <c r="R40" s="12" t="str">
         <f t="shared" si="3"/>
-        <v/>
+        <v>00100001</v>
       </c>
       <c r="S40" s="12" t="str">
         <f t="shared" si="4"/>
-        <v/>
+        <v>00100000</v>
       </c>
       <c r="T40" s="12" t="str">
         <f t="shared" ref="T40:U40" si="41">BIN2HEX(R40,2)</f>
-        <v>00</v>
+        <v>21</v>
       </c>
       <c r="U40" s="13" t="str">
         <f t="shared" si="41"/>
-        <v>00</v>
+        <v>20</v>
       </c>
       <c r="V40" s="12">
         <v>35</v>
@@ -3764,12 +3944,6 @@
     </row>
   </sheetData>
   <mergeCells count="16">
-    <mergeCell ref="A1:A2"/>
-    <mergeCell ref="B1:E1"/>
-    <mergeCell ref="F1:G1"/>
-    <mergeCell ref="H1:O1"/>
-    <mergeCell ref="Q1:W1"/>
-    <mergeCell ref="H2:O2"/>
     <mergeCell ref="C5:C16"/>
     <mergeCell ref="B31:B36"/>
     <mergeCell ref="B37:B38"/>
@@ -3780,6 +3954,12 @@
     <mergeCell ref="B28:B30"/>
     <mergeCell ref="C28:C30"/>
     <mergeCell ref="C31:C36"/>
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="B1:E1"/>
+    <mergeCell ref="F1:G1"/>
+    <mergeCell ref="H1:O1"/>
+    <mergeCell ref="Q1:W1"/>
+    <mergeCell ref="H2:O2"/>
   </mergeCells>
   <phoneticPr fontId="13" type="noConversion"/>
   <conditionalFormatting sqref="A1:A2">

</xml_diff>